<commit_message>
Figures, Tables, Supplementary Material
</commit_message>
<xml_diff>
--- a/paper/tables.xlsx
+++ b/paper/tables.xlsx
@@ -394,15 +394,13 @@
       <c r="B2" t="inlineStr">
         <is>
           <t>female: 67% (n = 320)
-male: 33% (n = 159)
-complete: n = 479</t>
+male: 33% (n = 159)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>female: 70% (n = 300)
-male: 30% (n = 127)
-complete: n = 427</t>
+male: 30% (n = 127)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -419,95 +417,89 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Age, years</t>
+          <t>Education</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>median: 43 [IQR: 32 - 53]
-range: 18 - 80
-complete: n = 479</t>
+          <t>non-tertiary: 63% (n = 302)
+tertiary: 37% (n = 176)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>median: 45 [IQR: 34 - 54]
-range: 18 - 95
-complete: n = 427</t>
+          <t>non-tertiary: 59% (n = 250)
+tertiary: 41% (n = 177)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ns (p = 0.31)</t>
+          <t>ns (p = 0.35)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>r = 0.048</t>
+          <t>V = 0.047</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Age, years</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>43 [IQR: 32 - 53]
+range: 18 - 80</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>45 [IQR: 34 - 54]
+range: 18 - 95</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ns (p = 0.31)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>r = 0.048</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>BMI before COVID-19</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>normal: 54% (n = 257)
 overweight: 28% (n = 135)
-obesity: 18% (n = 84)
-complete: n = 476</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
+obesity: 18% (n = 84)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>normal: 66% (n = 278)
 overweight: 25% (n = 104)
-obesity: 8.8% (n = 37)
-complete: n = 419</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+obesity: 8.8% (n = 37)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>p = 0.0011</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>V = 0.15</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Education</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>non-tertiary: 63% (n = 302)
-tertiary: 37% (n = 176)
-complete: n = 478</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>non-tertiary: 59% (n = 250)
-tertiary: 41% (n = 177)
-complete: n = 427</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>ns (p = 0.35)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>V = 0.047</t>
         </is>
       </c>
     </row>
@@ -522,8 +514,7 @@
           <t>employed: 83% (n = 398)
 unemployed: 8.4% (n = 40)
 leave: 1.7% (n = 8)
-retired: 6.9% (n = 33)
-complete: n = 479</t>
+retired: 6.9% (n = 33)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -531,8 +522,7 @@
           <t>employed: 81% (n = 348)
 unemployed: 9.4% (n = 40)
 leave: 1.9% (n = 8)
-retired: 7.3% (n = 31)
-complete: n = 427</t>
+retired: 7.3% (n = 31)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -549,205 +539,189 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Observation time</t>
+          <t>Autoimmunity</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>median: 180 [IQR: 130 - 220]
-range: 90 - 400
-complete: n = 479</t>
+          <t>6.7% (n = 32)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>median: 140 [IQR: 120 - 270]
-range: 90 - 390
-complete: n = 427</t>
+          <t>6.3% (n = 27)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>p = 0.0036</t>
+          <t>ns (p = 1)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>r = 0.12</t>
+          <t>V = 0.0072</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Comorbidity</t>
+          <t>Hypertension</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>49% (n = 237)
-complete: n = 479</t>
+          <t>11% (n = 51)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>43% (n = 185)
-complete: n = 427</t>
+          <t>8.4% (n = 36)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ns (p = 0.22)</t>
+          <t>ns (p = 0.46)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>V = 0.062</t>
+          <t>V = 0.038</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Hypertension</t>
+          <t>Pre-CoV depression/anxiety</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>11% (n = 51)
-complete: n = 479</t>
+          <t>5.4% (n = 26)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>8.4% (n = 36)
-complete: n = 427</t>
+          <t>5.2% (n = 22)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ns (p = 0.46)</t>
+          <t>ns (p = 1)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>V = 0.038</t>
+          <t>V = 0.0061</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Cardiovascular disease</t>
+          <t>Diabetes</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2.1% (n = 10)
-complete: n = 479</t>
+          <t>1.5% (n = 7)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3% (n = 13)
-complete: n = 427</t>
+          <t>0.23% (n = 1)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ns (p = 0.62)</t>
+          <t>ns (p = 0.26)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>V = 0.03</t>
+          <t>V = 0.065</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Diabetes</t>
+          <t>Freq. resp. infections</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1.5% (n = 7)
-complete: n = 479</t>
+          <t>6.7% (n = 32)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.23% (n = 1)
-complete: n = 427</t>
+          <t>3.3% (n = 14)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ns (p = 0.26)</t>
+          <t>ns (p = 0.1)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>V = 0.065</t>
+          <t>V = 0.077</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Pulmonary disease</t>
+          <t>Cardiovascular disease</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3.8% (n = 18)
-complete: n = 479</t>
+          <t>2.1% (n = 10)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2.8% (n = 12)
-complete: n = 427</t>
+          <t>3% (n = 13)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ns (p = 0.67)</t>
+          <t>ns (p = 0.62)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>V = 0.026</t>
+          <t>V = 0.03</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Gastrointestinal disease</t>
+          <t>Hay fever/allergy</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1.7% (n = 8)
-complete: n = 479</t>
+          <t>18% (n = 88)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.7% (n = 3)
-complete: n = 427</t>
+          <t>12% (n = 51)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ns (p = 0.46)</t>
+          <t>p = 0.045</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>V = 0.044</t>
+          <t>V = 0.089</t>
         </is>
       </c>
     </row>
@@ -759,14 +733,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2.1% (n = 10)
-complete: n = 479</t>
+          <t>2.1% (n = 10)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>4% (n = 17)
-complete: n = 427</t>
+          <t>4% (n = 17)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -783,207 +755,195 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Hay fever/allergy</t>
+          <t>Gastrointestinal disease</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>18% (n = 88)
-complete: n = 479</t>
+          <t>1.7% (n = 8)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>12% (n = 51)
-complete: n = 427</t>
+          <t>0.7% (n = 3)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>p = 0.045</t>
+          <t>ns (p = 0.46)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>V = 0.089</t>
+          <t>V = 0.044</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Autoimmunity</t>
+          <t>Pulmonary disease</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>6.7% (n = 32)
-complete: n = 479</t>
+          <t>3.8% (n = 18)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>6.3% (n = 27)
-complete: n = 427</t>
+          <t>2.8% (n = 12)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ns (p = 1)</t>
+          <t>ns (p = 0.67)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>V = 0.0072</t>
+          <t>V = 0.026</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Freq. resp. infections</t>
+          <t>Freq. bact. Infections</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>6.7% (n = 32)
-complete: n = 479</t>
+          <t>4.8% (n = 23)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>3.3% (n = 14)
-complete: n = 427</t>
+          <t>1.2% (n = 5)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ns (p = 0.1)</t>
+          <t>p = 0.016</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>V = 0.077</t>
+          <t>V = 0.1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Freq. bact. Infections</t>
+          <t>Pre-CoV sleep disorders</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4.8% (n = 23)
-complete: n = 479</t>
+          <t>3.5% (n = 17)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.2% (n = 5)
-complete: n = 427</t>
+          <t>4.7% (n = 20)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>p = 0.016</t>
+          <t>ns (p = 0.62)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>V = 0.1</t>
+          <t>V = 0.029</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Pre-CoV depression/anxiety</t>
+          <t>Daily medication</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>5.4% (n = 26)
-complete: n = 479</t>
+          <t>absent: 62% (n = 295)
+1 - 4 drugs: 37% (n = 175)
+5 drugs and more: 1.9% (n = 9)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>5.2% (n = 22)
-complete: n = 427</t>
+          <t>absent: 74% (n = 317)
+1 - 4 drugs: 25% (n = 106)
+5 drugs and more: 0.94% (n = 4)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>ns (p = 1)</t>
+          <t>p = 0.0024</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>V = 0.0061</t>
+          <t>V = 0.14</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Pre-CoV sleep disorders</t>
+          <t>Observation time</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3.5% (n = 17)
-complete: n = 479</t>
+          <t>180 [IQR: 130 - 220]
+range: 90 - 400</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>4.7% (n = 20)
-complete: n = 427</t>
+          <t>140 [IQR: 120 - 270]
+range: 90 - 390</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>ns (p = 0.62)</t>
+          <t>p = 0.0036</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>V = 0.029</t>
+          <t>r = 0.12</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Daily medication</t>
+          <t>Comorbidity</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>absent: 62% (n = 295)
-1 - 4 drugs: 37% (n = 175)
-5 drugs and more: 1.9% (n = 9)
-complete: n = 479</t>
+          <t>49% (n = 237)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>absent: 74% (n = 317)
-1 - 4 drugs: 25% (n = 106)
-5 drugs and more: 0.94% (n = 4)
-complete: n = 427</t>
+          <t>43% (n = 185)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>p = 0.0024</t>
+          <t>ns (p = 0.22)</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>V = 0.14</t>
+          <t>V = 0.062</t>
         </is>
       </c>
     </row>
@@ -1046,29 +1006,25 @@
       <c r="B2" t="inlineStr">
         <is>
           <t>female: 41% (n = 44)
-male: 59% (n = 64)
-complete: n = 108</t>
+male: 59% (n = 64)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>female: 67% (n = 18)
-male: 33% (n = 9)
-complete: n = 27</t>
+male: 33% (n = 9)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>female: 35% (n = 19)
-male: 65% (n = 36)
-complete: n = 55</t>
+male: 65% (n = 36)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>female: 27% (n = 7)
-male: 73% (n = 19)
-complete: n = 26</t>
+male: 73% (n = 19)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1090,30 +1046,26 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>median: 56 [IQR: 49 - 68]
-range: 19 - 87
-complete: n = 108</t>
+          <t>56 [IQR: 49 - 68]
+range: 19 - 87</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>median: 47 [IQR: 38 - 55]
-range: 19 - 70
-complete: n = 27</t>
+          <t>47 [IQR: 38 - 55]
+range: 19 - 70</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>median: 62 [IQR: 53 - 72]
-range: 27 - 87
-complete: n = 55</t>
+          <t>62 [IQR: 53 - 72]
+range: 27 - 87</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>median: 56 [IQR: 52 - 64]
-range: 44 - 79
-complete: n = 26</t>
+          <t>56 [IQR: 52 - 64]
+range: 44 - 79</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1137,32 +1089,28 @@
         <is>
           <t>normal: 39% (n = 42)
 overweight: 43% (n = 46)
-obesity: 19% (n = 20)
-complete: n = 108</t>
+obesity: 19% (n = 20)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>normal: 56% (n = 15)
 overweight: 33% (n = 9)
-obesity: 11% (n = 3)
-complete: n = 27</t>
+obesity: 11% (n = 3)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>normal: 29% (n = 16)
 overweight: 51% (n = 28)
-obesity: 20% (n = 11)
-complete: n = 55</t>
+obesity: 20% (n = 11)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>normal: 42% (n = 11)
 overweight: 35% (n = 9)
-obesity: 23% (n = 6)
-complete: n = 26</t>
+obesity: 23% (n = 6)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1184,26 +1132,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>75% (n = 81)
-complete: n = 108</t>
+          <t>75% (n = 81)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>41% (n = 11)
-complete: n = 27</t>
+          <t>41% (n = 11)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>85% (n = 47)
-complete: n = 55</t>
+          <t>85% (n = 47)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>88% (n = 23)
-complete: n = 26</t>
+          <t>88% (n = 23)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1220,31 +1164,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Metabolic disease</t>
+          <t>Cardiovascular disease</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>42% (n = 45)
-complete: n = 108</t>
+          <t>40% (n = 43)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>19% (n = 5)
-complete: n = 27</t>
+          <t>7.4% (n = 2)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>49% (n = 27)
-complete: n = 55</t>
+          <t>47% (n = 26)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>50% (n = 13)
-complete: n = 26</t>
+          <t>58% (n = 15)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1254,7 +1194,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>V = 0.27</t>
+          <t>V = 0.39</t>
         </is>
       </c>
     </row>
@@ -1266,26 +1206,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>27% (n = 29)
-complete: n = 108</t>
+          <t>27% (n = 29)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>7.4% (n = 2)
-complete: n = 27</t>
+          <t>7.4% (n = 2)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>27% (n = 15)
-complete: n = 55</t>
+          <t>27% (n = 15)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>46% (n = 12)
-complete: n = 26</t>
+          <t>46% (n = 12)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1302,72 +1238,64 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Cardiovascular disease</t>
+          <t>Pulmonary disease</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>40% (n = 43)
-complete: n = 108</t>
+          <t>19% (n = 20)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>7.4% (n = 2)
-complete: n = 27</t>
+          <t>11% (n = 3)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>47% (n = 26)
-complete: n = 55</t>
+          <t>22% (n = 12)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>58% (n = 15)
-complete: n = 26</t>
+          <t>19% (n = 5)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>p &lt; 0.001</t>
+          <t>p = 0.031</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>V = 0.39</t>
+          <t>V = 0.11</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Diabetes</t>
+          <t>Metabolic disease</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15% (n = 16)
-complete: n = 108</t>
+          <t>42% (n = 45)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>3.7% (n = 1)
-complete: n = 27</t>
+          <t>19% (n = 5)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>15% (n = 8)
-complete: n = 55</t>
+          <t>49% (n = 27)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>27% (n = 7)
-complete: n = 26</t>
+          <t>50% (n = 13)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1377,48 +1305,44 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>V = 0.23</t>
+          <t>V = 0.27</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Pulmonary disease</t>
+          <t>Diabetes</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>19% (n = 20)
-complete: n = 108</t>
+          <t>15% (n = 16)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>11% (n = 3)
-complete: n = 27</t>
+          <t>3.7% (n = 1)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>22% (n = 12)
-complete: n = 55</t>
+          <t>15% (n = 8)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>19% (n = 5)
-complete: n = 26</t>
+          <t>27% (n = 7)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>p = 0.031</t>
+          <t>p &lt; 0.001</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>V = 0.11</t>
+          <t>V = 0.23</t>
         </is>
       </c>
     </row>
@@ -1430,26 +1354,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>13% (n = 14)
-complete: n = 108</t>
+          <t>13% (n = 14)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0% (n = 0)
-complete: n = 27</t>
+          <t>0% (n = 0)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>20% (n = 11)
-complete: n = 55</t>
+          <t>20% (n = 11)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>12% (n = 3)
-complete: n = 26</t>
+          <t>12% (n = 3)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1471,26 +1391,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>9.3% (n = 10)
-complete: n = 108</t>
+          <t>9.3% (n = 10)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3.7% (n = 1)
-complete: n = 27</t>
+          <t>3.7% (n = 1)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>15% (n = 8)
-complete: n = 55</t>
+          <t>15% (n = 8)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3.8% (n = 1)
-complete: n = 26</t>
+          <t>3.8% (n = 1)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1512,26 +1428,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5.6% (n = 6)
-complete: n = 108</t>
+          <t>5.6% (n = 6)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0% (n = 0)
-complete: n = 27</t>
+          <t>0% (n = 0)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3.6% (n = 2)
-complete: n = 55</t>
+          <t>3.6% (n = 2)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>15% (n = 4)
-complete: n = 26</t>
+          <t>15% (n = 4)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">

</xml_diff>